<commit_message>
funciones para llenar trucks y containers. Falta dispararlos
</commit_message>
<xml_diff>
--- a/CMCP_Manufacturing/OutputCMPC.xlsx
+++ b/CMCP_Manufacturing/OutputCMPC.xlsx
@@ -2692,10 +2692,10 @@
         <v>2.0</v>
       </c>
       <c r="D75" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="E75" t="n">
-        <v>20.0</v>
+        <v>22.0</v>
       </c>
       <c r="F75" t="n">
         <v>0.0</v>
@@ -2707,10 +2707,10 @@
         <v>0.0</v>
       </c>
       <c r="I75" t="n">
-        <v>1510.9713529128549</v>
+        <v>1662.0684882041405</v>
       </c>
       <c r="J75" t="n">
-        <v>3076.7999999999997</v>
+        <v>3589.5999999999995</v>
       </c>
       <c r="K75" t="n">
         <v>6630.0</v>
@@ -5247,10 +5247,10 @@
         <v>3.0</v>
       </c>
       <c r="D148" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="E148" t="n">
-        <v>24.0</v>
+        <v>26.0</v>
       </c>
       <c r="F148" t="n">
         <v>0.0</v>
@@ -5262,10 +5262,10 @@
         <v>0.0</v>
       </c>
       <c r="I148" t="n">
-        <v>1730.7692307692307</v>
+        <v>1875.0</v>
       </c>
       <c r="J148" t="n">
-        <v>9600.0</v>
+        <v>10800.0</v>
       </c>
       <c r="K148" t="n">
         <v>3333.0</v>
@@ -7697,10 +7697,10 @@
         <v>1.0</v>
       </c>
       <c r="D218" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="E218" t="n">
-        <v>22.0</v>
+        <v>30.0</v>
       </c>
       <c r="F218" t="n">
         <v>0.0</v>
@@ -7712,10 +7712,10 @@
         <v>0.0</v>
       </c>
       <c r="I218" t="n">
-        <v>847.8461538461539</v>
+        <v>1156.1538461538462</v>
       </c>
       <c r="J218" t="n">
-        <v>10192.0</v>
+        <v>13104.0</v>
       </c>
       <c r="K218" t="n">
         <v>9406.0</v>
@@ -12737,10 +12737,10 @@
         <v>1.0</v>
       </c>
       <c r="D362" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="E362" t="n">
-        <v>16.0</v>
+        <v>18.0</v>
       </c>
       <c r="F362" t="n">
         <v>0.0</v>
@@ -12752,10 +12752,10 @@
         <v>0.0</v>
       </c>
       <c r="I362" t="n">
-        <v>788.24</v>
+        <v>886.77</v>
       </c>
       <c r="J362" t="n">
-        <v>6000.0</v>
+        <v>7000.0</v>
       </c>
       <c r="K362" t="n">
         <v>6486.0</v>
@@ -12772,10 +12772,10 @@
         <v>2.0</v>
       </c>
       <c r="D363" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="E363" t="n">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
       <c r="F363" t="n">
         <v>0.0</v>
@@ -12787,10 +12787,10 @@
         <v>0.0</v>
       </c>
       <c r="I363" t="n">
-        <v>689.71</v>
+        <v>788.24</v>
       </c>
       <c r="J363" t="n">
-        <v>7000.0</v>
+        <v>8000.0</v>
       </c>
       <c r="K363" t="n">
         <v>6486.0</v>
@@ -12877,10 +12877,10 @@
         <v>5.0</v>
       </c>
       <c r="D366" t="n">
-        <v>13.0</v>
+        <v>15.0</v>
       </c>
       <c r="E366" t="n">
-        <v>34.0</v>
+        <v>38.0</v>
       </c>
       <c r="F366" t="n">
         <v>0.0</v>
@@ -12892,10 +12892,10 @@
         <v>0.0</v>
       </c>
       <c r="I366" t="n">
-        <v>1952.5349999999999</v>
+        <v>2182.245</v>
       </c>
       <c r="J366" t="n">
-        <v>13000.0</v>
+        <v>15000.0</v>
       </c>
       <c r="K366" t="n">
         <v>6486.0</v>
@@ -12912,10 +12912,10 @@
         <v>6.0</v>
       </c>
       <c r="D367" t="n">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="E367" t="n">
-        <v>48.0</v>
+        <v>50.0</v>
       </c>
       <c r="F367" t="n">
         <v>0.0</v>
@@ -12927,10 +12927,10 @@
         <v>0.0</v>
       </c>
       <c r="I367" t="n">
-        <v>2756.5199999999995</v>
+        <v>2871.3749999999995</v>
       </c>
       <c r="J367" t="n">
-        <v>18000.0</v>
+        <v>19000.0</v>
       </c>
       <c r="K367" t="n">
         <v>6486.0</v>
@@ -15292,10 +15292,10 @@
         <v>2.0</v>
       </c>
       <c r="D435" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="E435" t="n">
-        <v>12.0</v>
+        <v>14.0</v>
       </c>
       <c r="F435" t="n">
         <v>0.0</v>
@@ -15307,10 +15307,10 @@
         <v>0.0</v>
       </c>
       <c r="I435" t="n">
-        <v>674.946431822347</v>
+        <v>787.4375037927381</v>
       </c>
       <c r="J435" t="n">
-        <v>2637.6295384615387</v>
+        <v>3297.0369230769234</v>
       </c>
       <c r="K435" t="n">
         <v>3271.4175732133326</v>
@@ -15327,10 +15327,10 @@
         <v>3.0</v>
       </c>
       <c r="D436" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="E436" t="n">
-        <v>18.0</v>
+        <v>20.0</v>
       </c>
       <c r="F436" t="n">
         <v>0.0</v>
@@ -15342,10 +15342,10 @@
         <v>0.0</v>
       </c>
       <c r="I436" t="n">
-        <v>1083.0729147985214</v>
+        <v>1203.414349776135</v>
       </c>
       <c r="J436" t="n">
-        <v>5690.4030085470085</v>
+        <v>6828.4836102564095</v>
       </c>
       <c r="K436" t="n">
         <v>3271.4175732133326</v>
@@ -17777,10 +17777,10 @@
         <v>1.0</v>
       </c>
       <c r="D506" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="E506" t="n">
-        <v>20.0</v>
+        <v>22.0</v>
       </c>
       <c r="F506" t="n">
         <v>0.0</v>
@@ -17792,10 +17792,10 @@
         <v>0.0</v>
       </c>
       <c r="I506" t="n">
-        <v>1040.897435897436</v>
+        <v>1144.9871794871794</v>
       </c>
       <c r="J506" t="n">
-        <v>7560.0</v>
+        <v>8820.0</v>
       </c>
       <c r="K506" t="n">
         <v>7000.0</v>

</xml_diff>